<commit_message>
Add venv to .gitignore
</commit_message>
<xml_diff>
--- a/知識點鏈結/課綱.xlsx
+++ b/知識點鏈結/課綱.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="95">
   <si>
     <t>大單元</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t>積分的應用</t>
+  </si>
+  <si>
+    <t>generator_key</t>
+  </si>
+  <si>
+    <t>logarithms</t>
   </si>
 </sst>
 </file>
@@ -371,10 +377,10 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -656,10 +662,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D67"/>
+  <dimension ref="A1:E67"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.45" x14ac:dyDescent="0.4"/>
@@ -667,187 +673,194 @@
     <col min="1" max="1" width="12.75" customWidth="1"/>
     <col min="2" max="2" width="21.4140625" customWidth="1"/>
     <col min="3" max="3" width="40.4140625" customWidth="1"/>
-    <col min="4" max="4" width="61.75" customWidth="1"/>
+    <col min="4" max="4" width="76.6640625" customWidth="1"/>
+    <col min="5" max="5" width="26.25" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2" s="2" t="s">
+      <c r="E1" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="3" t="s">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A3" s="3"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4" s="2"/>
-      <c r="B4" s="2" t="s">
+      <c r="E3" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A4" s="3"/>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="D4" s="3"/>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="3" t="s">
+      <c r="D4" s="2"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="3"/>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6" s="2"/>
-      <c r="B6" s="2"/>
-      <c r="C6" s="3" t="s">
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D6" s="3"/>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7" s="2"/>
-      <c r="B7" s="2" t="s">
+      <c r="D6" s="2"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A7" s="3"/>
+      <c r="B7" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="D7" s="3"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8" s="2"/>
-      <c r="B8" s="2"/>
-      <c r="C8" s="3" t="s">
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A8" s="3"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="3"/>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A9" s="2"/>
-      <c r="B9" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A9" s="3"/>
+      <c r="B9" s="3"/>
       <c r="C9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="3"/>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="3" t="s">
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="3"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2" t="s">
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A11" s="3"/>
+      <c r="B11" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="3"/>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="3" t="s">
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D12" s="3"/>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="3" t="s">
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A13" s="3"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="3"/>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="3" t="s">
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="D14" s="3"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="3" t="s">
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D15" s="3"/>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="3" t="s">
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="D16" s="3"/>
+      <c r="D16" s="2"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="3" t="s">
+      <c r="A17" s="3"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D17" s="3"/>
+      <c r="D17" s="2"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="3" t="s">
+      <c r="A18" s="3"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D18" s="3"/>
+      <c r="D18" s="2"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="3" t="s">
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D19" s="3"/>
+      <c r="D19" s="2"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2" t="s">
+      <c r="A20" s="3"/>
+      <c r="B20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C20" s="3" t="s">
+      <c r="C20" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D20" s="1" t="s">
@@ -855,9 +868,9 @@
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="3" t="s">
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D21" s="1" t="s">
@@ -865,9 +878,9 @@
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A22" s="2"/>
-      <c r="B22" s="2"/>
-      <c r="C22" s="3" t="s">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="2" t="s">
         <v>36</v>
       </c>
       <c r="D22" s="1" t="s">
@@ -875,9 +888,9 @@
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A23" s="2"/>
-      <c r="B23" s="2"/>
-      <c r="C23" s="3" t="s">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="2" t="s">
         <v>37</v>
       </c>
       <c r="D23" s="1" t="s">
@@ -885,13 +898,13 @@
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A24" s="2" t="s">
+      <c r="A24" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="3" t="s">
+      <c r="C24" s="2" t="s">
         <v>57</v>
       </c>
       <c r="D24" s="1" t="s">
@@ -899,9 +912,9 @@
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A25" s="2"/>
-      <c r="B25" s="2"/>
-      <c r="C25" s="3" t="s">
+      <c r="A25" s="3"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D25" s="1" t="s">
@@ -909,9 +922,9 @@
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A26" s="2"/>
-      <c r="B26" s="2"/>
-      <c r="C26" s="3" t="s">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="2" t="s">
         <v>61</v>
       </c>
       <c r="D26" s="1" t="s">
@@ -919,9 +932,9 @@
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A27" s="2"/>
-      <c r="B27" s="2"/>
-      <c r="C27" s="3" t="s">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="2" t="s">
         <v>63</v>
       </c>
       <c r="D27" s="1" t="s">
@@ -929,27 +942,27 @@
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A28" s="2"/>
-      <c r="B28" s="2" t="s">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="3"/>
+      <c r="D28" s="2"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A29" s="2"/>
-      <c r="B29" s="2"/>
-      <c r="C29" s="3" t="s">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="D29" s="3"/>
+      <c r="D29" s="2"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A30" s="2"/>
-      <c r="B30" s="2"/>
-      <c r="C30" s="3" t="s">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="2" t="s">
         <v>41</v>
       </c>
       <c r="D30" s="1" t="s">
@@ -957,9 +970,9 @@
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A31" s="2"/>
-      <c r="B31" s="2"/>
-      <c r="C31" s="3" t="s">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="2" t="s">
         <v>43</v>
       </c>
       <c r="D31" s="1" t="s">
@@ -967,9 +980,9 @@
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A32" s="2"/>
-      <c r="B32" s="2"/>
-      <c r="C32" s="3" t="s">
+      <c r="A32" s="3"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="2" t="s">
         <v>45</v>
       </c>
       <c r="D32" s="1" t="s">
@@ -977,296 +990,296 @@
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A33" s="2"/>
-      <c r="B33" s="2" t="s">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C33" s="3" t="s">
+      <c r="C33" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D33" s="3"/>
+      <c r="D33" s="2"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A34" s="2"/>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3" t="s">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="3"/>
+      <c r="D34" s="2"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="2"/>
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
       <c r="C35" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="3"/>
+      <c r="D35" s="2"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A36" s="2"/>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3" t="s">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="D36" s="3"/>
+      <c r="D36" s="2"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A37" s="2"/>
-      <c r="B37" s="2"/>
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
       <c r="C37" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="D37" s="3"/>
+      <c r="D37" s="2"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A38" s="2"/>
-      <c r="B38" s="2"/>
-      <c r="C38" s="3" t="s">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="D38" s="3"/>
+      <c r="D38" s="2"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A39" s="2"/>
-      <c r="B39" s="2"/>
-      <c r="C39" s="3" t="s">
+      <c r="A39" s="3"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="D39" s="3"/>
+      <c r="D39" s="2"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="3" t="s">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="D40" s="3"/>
+      <c r="D40" s="2"/>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="3" t="s">
+      <c r="A41" s="3"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="2" t="s">
         <v>56</v>
       </c>
-      <c r="D41" s="3"/>
+      <c r="D41" s="2"/>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A42" s="2"/>
-      <c r="B42" s="3" t="s">
+      <c r="A42" s="3"/>
+      <c r="B42" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="C42" s="3" t="s">
+      <c r="C42" s="2" t="s">
         <v>66</v>
       </c>
-      <c r="D42" s="3"/>
+      <c r="D42" s="2"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="3" t="s">
+      <c r="C43" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="3"/>
+      <c r="D43" s="2"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
       <c r="C44" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="D44" s="3"/>
+      <c r="D44" s="2"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A45" s="2"/>
-      <c r="B45" s="2"/>
-      <c r="C45" s="3" t="s">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="D45" s="3"/>
+      <c r="D45" s="2"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A46" s="2"/>
-      <c r="B46" s="2"/>
-      <c r="C46" s="3" t="s">
+      <c r="A46" s="3"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="D46" s="3"/>
+      <c r="D46" s="2"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A47" s="2"/>
-      <c r="B47" s="2"/>
-      <c r="C47" s="3" t="s">
+      <c r="A47" s="3"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D47" s="3"/>
+      <c r="D47" s="2"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A48" s="2"/>
-      <c r="B48" s="2"/>
-      <c r="C48" s="3" t="s">
+      <c r="A48" s="3"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D48" s="3"/>
+      <c r="D48" s="2"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A49" s="2"/>
-      <c r="B49" s="2"/>
-      <c r="C49" s="3" t="s">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D49" s="3"/>
+      <c r="D49" s="2"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A50" s="2"/>
-      <c r="B50" s="2"/>
-      <c r="C50" s="3" t="s">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="D50" s="3"/>
+      <c r="D50" s="2"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A51" s="2"/>
-      <c r="B51" s="2"/>
-      <c r="C51" s="3" t="s">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D51" s="3"/>
+      <c r="D51" s="2"/>
     </row>
     <row r="52" spans="1:4" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A52" s="2"/>
-      <c r="B52" s="2"/>
-      <c r="C52" s="3" t="s">
+      <c r="A52" s="3"/>
+      <c r="B52" s="3"/>
+      <c r="C52" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="D52" s="3"/>
+      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A53" s="2"/>
-      <c r="B53" s="2"/>
-      <c r="C53" s="3" t="s">
+      <c r="A53" s="3"/>
+      <c r="B53" s="3"/>
+      <c r="C53" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D53" s="3"/>
+      <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A54" s="2"/>
-      <c r="B54" s="2" t="s">
+      <c r="A54" s="3"/>
+      <c r="B54" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C54" s="3" t="s">
+      <c r="C54" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="D54" s="3"/>
+      <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A55" s="2"/>
-      <c r="B55" s="2"/>
-      <c r="C55" s="3" t="s">
+      <c r="A55" s="3"/>
+      <c r="B55" s="3"/>
+      <c r="C55" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D55" s="3"/>
+      <c r="D55" s="2"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A56" s="2"/>
-      <c r="B56" s="2"/>
-      <c r="C56" s="3" t="s">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3"/>
+      <c r="C56" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="D56" s="3"/>
+      <c r="D56" s="2"/>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A57" s="2"/>
-      <c r="B57" s="2"/>
+      <c r="A57" s="3"/>
+      <c r="B57" s="3"/>
       <c r="C57" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="D57" s="3"/>
+      <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A58" s="2"/>
-      <c r="B58" s="2"/>
-      <c r="C58" s="3" t="s">
+      <c r="A58" s="3"/>
+      <c r="B58" s="3"/>
+      <c r="C58" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="D58" s="3"/>
+      <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A59" s="2"/>
-      <c r="B59" s="2"/>
+      <c r="A59" s="3"/>
+      <c r="B59" s="3"/>
       <c r="C59" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="D59" s="3"/>
+      <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A60" s="2"/>
-      <c r="B60" s="2"/>
-      <c r="C60" s="3" t="s">
+      <c r="A60" s="3"/>
+      <c r="B60" s="3"/>
+      <c r="C60" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="D60" s="3"/>
+      <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A61" s="2"/>
-      <c r="B61" s="2"/>
-      <c r="C61" s="3" t="s">
+      <c r="A61" s="3"/>
+      <c r="B61" s="3"/>
+      <c r="C61" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D61" s="3"/>
+      <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" ht="25.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A62" s="2"/>
-      <c r="B62" s="2"/>
-      <c r="C62" s="3" t="s">
+      <c r="A62" s="3"/>
+      <c r="B62" s="3"/>
+      <c r="C62" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="D62" s="3"/>
+      <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A63" s="2"/>
-      <c r="B63" s="2" t="s">
+      <c r="A63" s="3"/>
+      <c r="B63" s="3" t="s">
         <v>65</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="D63" s="3"/>
+      <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A64" s="2"/>
-      <c r="B64" s="2"/>
+      <c r="A64" s="3"/>
+      <c r="B64" s="3"/>
       <c r="C64" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="D64" s="3"/>
+      <c r="D64" s="2"/>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A65" s="2"/>
-      <c r="B65" s="2"/>
-      <c r="C65" s="3" t="s">
+      <c r="A65" s="3"/>
+      <c r="B65" s="3"/>
+      <c r="C65" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D65" s="3"/>
+      <c r="D65" s="2"/>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A66" s="2"/>
-      <c r="B66" s="2"/>
-      <c r="C66" s="3" t="s">
+      <c r="A66" s="3"/>
+      <c r="B66" s="3"/>
+      <c r="C66" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="D66" s="3"/>
+      <c r="D66" s="2"/>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A67" s="2"/>
-      <c r="B67" s="2"/>
-      <c r="C67" s="3" t="s">
+      <c r="A67" s="3"/>
+      <c r="B67" s="3"/>
+      <c r="C67" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="D67" s="3"/>
+      <c r="D67" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">

</xml_diff>